<commit_message>
cambie el swing por un nimbus, para que se vea mas actual, y modifique para que se pueda exportar del proyecto al excel, y no se cambien nunca los datos a menos que yo lo haga manualmente, al cerrar proyectos
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -26,25 +26,25 @@
     <t>Total Producto</t>
   </si>
   <si>
-    <t>Pagado</t>
+    <t>Total Cuotas</t>
   </si>
   <si>
-    <t>Deuda</t>
+    <t>Valor Cuota</t>
   </si>
   <si>
-    <t>Nicolas Davalos</t>
+    <t>Cuotas Pagadas</t>
   </si>
   <si>
-    <t>------</t>
+    <t>Monto Pagado</t>
   </si>
   <si>
-    <t>quincenal</t>
+    <t>Deuda Restante</t>
   </si>
   <si>
-    <t>Kevin Nogueroles</t>
+    <t>Mauricio</t>
   </si>
   <si>
-    <t>-----</t>
+    <t>L</t>
   </si>
   <si>
     <t>Quincenal</t>
@@ -55,7 +55,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -63,13 +63,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="18"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,86 +100,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.6796875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="5.078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.45703125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.265625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="7.6328125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="8.84375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="8.99609375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="4.48046875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.70703125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.46875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.8203125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="15.33984375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.53515625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="15.6171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s" s="1">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s" s="1">
         <v>5</v>
+      </c>
+      <c r="G1" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>920000.0</v>
+        <v>1500000.0</v>
       </c>
       <c r="E2" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>130000.0</v>
+      </c>
+      <c r="G2" t="n" s="0">
         <v>0.0</v>
       </c>
-      <c r="F2" t="n" s="0">
-        <v>920000.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>1200000.0</v>
-      </c>
-      <c r="E3" t="n" s="0">
+      <c r="H2" t="n" s="0">
         <v>0.0</v>
       </c>
-      <c r="F3" t="n" s="0">
-        <v>1200000.0</v>
+      <c r="I2" t="n" s="0">
+        <v>1500000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Actualizar README y archivo de clientes
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Nombre</t>
   </si>
@@ -41,19 +41,61 @@
     <t>Nicolas</t>
   </si>
   <si>
+    <t>Davalos</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>quincenal</t>
+  </si>
+  <si>
+    <t>Tv usado</t>
+  </si>
+  <si>
+    <t>[{"numeroCuota":1,"montoOriginal":115000.0,"montoPagado":115000.0,"fechaVencimiento":"2025-07-03","fechaPago":"2025-07-03","isFaltante":false},{"numeroCuota":2,"montoOriginal":115000.0,"montoPagado":0.0,"fechaVencimiento":"2025-07-17","fechaPago":"","isFaltante":false},{"numeroCuota":3,"montoOriginal":115000.0,"montoPagado":0.0,"fechaVencimiento":"2025-07-31","fechaPago":"","isFaltante":false},{"numeroCuota":4,"montoOriginal":115000.0,"montoPagado":0.0,"fechaVencimiento":"2025-08-14","fechaPago":"","isFaltante":false},{"numeroCuota":5,"montoOriginal":115000.0,"montoPagado":0.0,"fechaVencimiento":"2025-08-28","fechaPago":"","isFaltante":false},{"numeroCuota":6,"montoOriginal":115000.0,"montoPagado":0.0,"fechaVencimiento":"2025-09-11","fechaPago":"","isFaltante":false},{"numeroCuota":7,"montoOriginal":115000.0,"montoPagado":0.0,"fechaVencimiento":"2025-09-25","fechaPago":"","isFaltante":false},{"numeroCuota":8,"montoOriginal":115000.0,"montoPagado":0.0,"fechaVencimiento":"2025-10-09","fechaPago":"","isFaltante":false}]</t>
+  </si>
+  <si>
+    <t>Kevincito</t>
+  </si>
+  <si>
+    <t>Chagaray</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>mensual</t>
+  </si>
+  <si>
+    <t>Celular</t>
+  </si>
+  <si>
+    <t>[{"numeroCuota":1,"montoOriginal":90000.0,"montoPagado":90000.0,"fechaVencimiento":"2025-07-03","fechaPago":"2025-07-03","isFaltante":false},{"numeroCuota":2,"montoOriginal":90000.0,"montoPagado":50000.0,"fechaVencimiento":"2025-08-03","fechaPago":"","isFaltante":false},{"numeroCuota":3,"montoOriginal":90000.0,"montoPagado":0.0,"fechaVencimiento":"2025-09-03","fechaPago":"","isFaltante":false}]</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
     <t>Nogueroles</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>quincenal</t>
-  </si>
-  <si>
-    <t>Televisor 75"</t>
-  </si>
-  <si>
-    <t>[{"numeroCuota":1,"montoOriginal":275000.0,"montoPagado":275000.0,"fechaVencimiento":"2025-07-03","fechaPago":"2025-07-03","isFaltante":false},{"numeroCuota":2,"montoOriginal":275000.0,"montoPagado":275000.0,"fechaVencimiento":"2025-07-17","fechaPago":"2025-07-03","isFaltante":false},{"numeroCuota":3,"montoOriginal":275000.0,"montoPagado":122222.0,"fechaVencimiento":"2025-07-31","fechaPago":"","isFaltante":false},{"numeroCuota":4,"montoOriginal":275000.0,"montoPagado":0.0,"fechaVencimiento":"2025-08-14","fechaPago":"","isFaltante":false},{"numeroCuota":5,"montoOriginal":275000.0,"montoPagado":0.0,"fechaVencimiento":"2025-08-28","fechaPago":"","isFaltante":false},{"numeroCuota":6,"montoOriginal":275000.0,"montoPagado":0.0,"fechaVencimiento":"2025-09-11","fechaPago":"","isFaltante":false}]</t>
+    <t>Tv</t>
+  </si>
+  <si>
+    <t>[{"numeroCuota":1,"montoOriginal":150000.0,"montoPagado":150000.0,"fechaVencimiento":"2025-07-03","fechaPago":"2025-07-03","isFaltante":false},{"numeroCuota":2,"montoOriginal":150000.0,"montoPagado":150000.0,"fechaVencimiento":"2025-07-17","fechaPago":"2025-07-03","isFaltante":false},{"numeroCuota":3,"montoOriginal":150000.0,"montoPagado":100000.0,"fechaVencimiento":"2025-07-31","fechaPago":"","isFaltante":false},{"numeroCuota":4,"montoOriginal":150000.0,"montoPagado":0.0,"fechaVencimiento":"2025-08-14","fechaPago":"","isFaltante":false},{"numeroCuota":5,"montoOriginal":150000.0,"montoPagado":0.0,"fechaVencimiento":"2025-08-28","fechaPago":"","isFaltante":false},{"numeroCuota":6,"montoOriginal":150000.0,"montoPagado":0.0,"fechaVencimiento":"2025-09-11","fechaPago":"","isFaltante":false},{"numeroCuota":7,"montoOriginal":150000.0,"montoPagado":0.0,"fechaVencimiento":"2025-09-25","fechaPago":"","isFaltante":false},{"numeroCuota":8,"montoOriginal":150000.0,"montoPagado":0.0,"fechaVencimiento":"2025-10-09","fechaPago":"","isFaltante":false}]</t>
+  </si>
+  <si>
+    <t>Florencia</t>
+  </si>
+  <si>
+    <t>Microhondas</t>
+  </si>
+  <si>
+    <t>[{"numeroCuota":1,"montoOriginal":50000.0,"montoPagado":0.0,"fechaVencimiento":"2025-07-03","fechaPago":"","isFaltante":false},{"numeroCuota":2,"montoOriginal":50000.0,"montoPagado":0.0,"fechaVencimiento":"2025-08-03","fechaPago":"","isFaltante":false},{"numeroCuota":3,"montoOriginal":50000.0,"montoPagado":0.0,"fechaVencimiento":"2025-09-03","fechaPago":"","isFaltante":false},{"numeroCuota":4,"montoOriginal":50000.0,"montoPagado":0.0,"fechaVencimiento":"2025-10-03","fechaPago":"","isFaltante":false}]</t>
   </si>
 </sst>
 </file>
@@ -117,17 +159,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="8.546875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="9.26171875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.2890625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="4.48046875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.70703125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.69921875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.82421875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.578125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.3203125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="255.0" customWidth="true" bestFit="true"/>
@@ -176,13 +218,91 @@
         <v>12</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>1650000.0</v>
+        <v>920000.0</v>
       </c>
       <c r="G2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>270000.0</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>1200000.0</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>200000.0</v>
+      </c>
+      <c r="G5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>